<commit_message>
2nd commit (with analysis code)
</commit_message>
<xml_diff>
--- a/data/4. data_ready_for_analysis/ready_for_analysis.xlsx
+++ b/data/4. data_ready_for_analysis/ready_for_analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python advenced\my_final_reposatory\data\4. data_ready_for_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python advenced\final-project\data\4. data_ready_for_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FEBDF-D6B2-4EAC-AF63-92835FFBBBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AA289-4A99-46C4-AE84-B1872F9C412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Gamma</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>Theta</t>
-  </si>
-  <si>
-    <t>Delta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>AF7</t>
   </si>
@@ -52,16 +37,51 @@
   </si>
   <si>
     <t>TP9</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>DELTA</t>
+  </si>
+  <si>
+    <t>THETA</t>
+  </si>
+  <si>
+    <t>ALPHA</t>
+  </si>
+  <si>
+    <t>BETA</t>
+  </si>
+  <si>
+    <t>GAMMA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,14 +104,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{F2BE3169-C5A3-4F31-BF63-D1220DEA117F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -372,7 +403,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -381,17 +412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -407,8 +441,8 @@
       <c r="D2">
         <v>184</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -424,8 +458,8 @@
       <c r="D3">
         <v>105</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -441,8 +475,8 @@
       <c r="D4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,8 +492,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>1</v>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,8 +509,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>0</v>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done (missing tests)
</commit_message>
<xml_diff>
--- a/data/4. data_ready_for_analysis/ready_for_analysis.xlsx
+++ b/data/4. data_ready_for_analysis/ready_for_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python advenced\final-project\data\4. data_ready_for_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AA289-4A99-46C4-AE84-B1872F9C412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D783AF5-E686-4BD5-91D0-435C894AA9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,38 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>AF7</t>
-  </si>
-  <si>
-    <t>AF8</t>
-  </si>
-  <si>
-    <t>TP10</t>
-  </si>
-  <si>
-    <t>TP9</t>
-  </si>
-  <si>
-    <t>wave</t>
-  </si>
-  <si>
-    <t>DELTA</t>
-  </si>
-  <si>
-    <t>THETA</t>
-  </si>
-  <si>
-    <t>ALPHA</t>
-  </si>
-  <si>
-    <t>BETA</t>
-  </si>
-  <si>
-    <t>GAMMA</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,7 +372,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -412,106 +381,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>178</v>
-      </c>
-      <c r="B2">
-        <v>181</v>
-      </c>
-      <c r="C2">
-        <v>172</v>
-      </c>
-      <c r="D2">
-        <v>184</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>93</v>
-      </c>
-      <c r="B3">
-        <v>91</v>
-      </c>
-      <c r="C3">
-        <v>91</v>
-      </c>
-      <c r="D3">
-        <v>105</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>